<commit_message>
Added mini PEKKA team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,6 +529,38 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>mini PEKKA</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Federico Leonardi | Rita Levi’s</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Davide  Rosa` | Hellas Lazio</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Lorenzo Casari | Nazzzionale ferrovieri</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Mattia Festi | SHARK ATTACK</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Matteo Gatti | demobusters</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Sara Isabel Pisoni team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -657,6 +657,38 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Sara Isabel Pisoni</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Elia Battisti | U.SGUARNA</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Filippo Benetti | I Magnifici</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Andrea Conzatti | FC SAVIGNANO</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Lorenzo Rossi | Power Ginger</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Andreas Galli | SdrumALA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Simone Martini team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -689,6 +689,38 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Simone Martini</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Elia Battisti | U.SGUARNA</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Simone Martini | Hellas Lazio</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Michele Merighi | Clitoriders</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Filippo Benetti | I Magnifici</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Davide  Bazzano | IMONTAGNA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Los Ripudiatos team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -721,6 +721,38 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Los Ripudiatos</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Matteo Zanlucchi | SBARX</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Daniele Feltrinelli | Rita Levi’s</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Andrea Conzatti | FC SAVIGNANO</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Alessio Farinati | Pinguini Trentini</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Giovanni  Lasta | 4SINS</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Lorenzo Zuani team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -785,6 +785,38 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Lorenzo Zuani</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Elia Barozzi | I Magnifici</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Alessio Bragagna | SHARK ATTACK</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Federico Nicolodi | U.SGUARNA</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Filippo Benetti | I Magnifici</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Nicholas Marzadro | SBARX</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added James Trivette team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -849,6 +849,38 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>James Trivette</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Federico Zoller | GREP</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Federico Manica | IMONTAGNA</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Alessandro Maffei | FC SAVIGNANO</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Federico Nicolodi | U.SGUARNA</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Alessio Debiasi | Mai una gioia</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added APERITIVO AL MOZART team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1137,6 +1137,38 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>APERITIVO AL MOZART</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Samuele Kettmaier | A.C.DENTI</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Andrea Conzatti | FC SAVIGNANO</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Andrea Menolli | SdrumALA</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Giacomo  Gasparini  | Mai una gioia</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Alessio Zandonai | SBARX</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Biker mice team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1201,6 +1201,38 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Biker mice</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Nicolas Giordani  | FC SAVIGNANO</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Federico Fasanelli | SBARX</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Matteo Diener | U.SGUARNA</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Filippo Benetti | I Magnifici</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Alessio Debiasi | Mai una gioia</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added ah ma è ronco  team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1265,6 +1265,38 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ah ma è ronco </t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Matteo Zanlucchi | SBARX</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Carlo  Stedile | Mai una gioia</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Nicolo  Speziali | FC GORILLAZ</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Matteo Simoncelli | IMONTAGNA</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Francesco Cristoforetti | Vigili del Fusto</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Jacopo Chemini team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1297,6 +1297,38 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Jacopo Chemini</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Stefano  Tita | Clitoriders</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Daniel Pedrotti | IMONTAGNA</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Michele Merighi | Clitoriders</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>maikol  azocar | Mai una gioia</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Emanuele Toss | 4SINS</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Senia Lucrezia team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1329,6 +1329,38 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Senia Lucrezia</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Elia Battisti | U.SGUARNA</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Daniel Pedrotti | IMONTAGNA</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Michele Merighi | Clitoriders</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Gabriele Verona | CGB Gamberoni</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Gianni Sala | FC SALAGIARDINI</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Thomas Cavagna team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1457,6 +1457,38 @@
         </is>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Thomas Cavagna</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Thomas Debiasi | Mai una gioia</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Thomas Cavagna | Mai una gioia</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Luca Frasca | Clitoriders</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Federico Nicolodi | U.SGUARNA</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Davide  Bazzano | IMONTAGNA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Jasmine Scottini team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1585,6 +1585,38 @@
         </is>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Jasmine Scottini</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Elia Battisti | U.SGUARNA</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Federico Fasanelli | SBARX</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Filippo Benetti | I Magnifici</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Luca Frasca | Clitoriders</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Francesco Cristoforetti | Vigili del Fusto</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Michele Leonardi  team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1617,6 +1617,38 @@
         </is>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Michele Leonardi </t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Elia Battisti | U.SGUARNA</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Filippo Benetti | I Magnifici</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Matteo Diener | U.SGUARNA</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Luca Tonolli | Rita Levi’s</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Sayf Brik | A.C.DENTI</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Nicolas Giordani team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1681,6 +1681,38 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Nicolas Giordani</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Elia Battisti | U.SGUARNA</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Filippo Benetti | I Magnifici</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Federico Mortillaro | Clitoriders</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Federico  Zanini | A.C.DENTI</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Geremia  Carollo | FC SAVIGNANO</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Michela Menghini team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1713,6 +1713,38 @@
         </is>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Michela Menghini</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Nicolas Giordani  | FC SAVIGNANO</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Andrea Conzatti | FC SAVIGNANO</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Matteo Mazzola | GREP</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Alessio Farinati | Pinguini Trentini</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Emanuele  valduga | wanda tim</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Matteo Alberti team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1809,6 +1809,38 @@
         </is>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Matteo Alberti</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Thomas Debiasi | Mai una gioia</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Nadir  chtioui | Mai una gioia</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Michael Bertè  | A.C.DENTI</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Andreas Galli | SdrumALA</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Lorenzo Zuani | I Magnifici</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Leo Parisi  team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1841,6 +1841,38 @@
         </is>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Leo Parisi </t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Daniele Dalbosco | IMONTAGNA</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Leonardo Viola | SHARK ATTACK</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Geremia  Carollo | FC SAVIGNANO</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Luca Frasca | Clitoriders</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Moris Benedetti | Gli Introvabili</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Giacomo Gasparini team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1905,6 +1905,38 @@
         </is>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Giacomo Gasparini</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Mattia Kaiserman | Gli Introvabili</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Federico  Andreis | IMONTAGNA</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Michele Merighi | Clitoriders</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Geremia  Carollo | FC SAVIGNANO</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Alessio Delli Compagni | SdrumALA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added I magnifici 2.0 team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1937,6 +1937,38 @@
         </is>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>I magnifici 2.0</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Stefano  Tita | Clitoriders</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Alessio Bragagna | SHARK ATTACK</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Pietro  Gasparini | Mai una gioia</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Geremia  Carollo | FC SAVIGNANO</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Mattia Tezzele | U.SGUARNA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Danny Giordani team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2001,6 +2001,38 @@
         </is>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Danny Giordani</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Nicolas Giordani  | FC SAVIGNANO</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Danny Giordani | I Magnifici</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Luca Frasca | Clitoriders</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Alessandro Maffei | FC SAVIGNANO</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Gentian Capa | Power Ginger</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Giovanni Simoncelli team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2065,6 +2065,38 @@
         </is>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Giovanni Simoncelli</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Stefano  Tita | Clitoriders</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Daniele Feltrinelli | Rita Levi’s</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Sebastiano Zoller | CGB Gamberoni</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Andrea  Pedrotti | IMONTAGNA</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Alessandro Galvagni | Hellas Lazio</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Riccardo Briosi team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2097,6 +2097,38 @@
         </is>
       </c>
     </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Riccardo Briosi</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Riccardo Versini | Modium</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Andrea Conzatti | FC SAVIGNANO</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Luca Frasca | Clitoriders</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Gianni Sala | FC SALAGIARDINI</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Christian Torboli | 4SINS</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Francesco Passuello team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2129,6 +2129,38 @@
         </is>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Francesco Passuello</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Gabriel Melis | demobusters</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Mattia Baldessarini | SHARK ATTACK</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Federico Mortillaro | Clitoriders</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Mattia Tezzele | U.SGUARNA</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Thomas Pontillo | Gli Introvabili</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Bruno 🐻 team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2257,6 +2257,38 @@
         </is>
       </c>
     </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Bruno 🐻</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Nicolas Giordani  | FC SAVIGNANO</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Marco Sala | IMONTAGNA</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Danny Giordani | I Magnifici</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Riccardo Zaffoni | U.SGUARNA</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Alessio Debiasi | Mai una gioia</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Davide Scarperi team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2289,6 +2289,38 @@
         </is>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Davide Scarperi</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Alessandro  Ruele  | FC GORILLAZ</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Andrea Conzatti | FC SAVIGNANO</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Alessio Bragagna | SHARK ATTACK</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Daniel Pedrotti | IMONTAGNA</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Emanuele  valduga | wanda tim</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Davide Raffaelli  team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2321,6 +2321,38 @@
         </is>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Davide Raffaelli </t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Alberto Cerisara | SHARK ATTACK</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Daniele Feller | GREP</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Matteo Simoncelli | IMONTAGNA</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Leonardo Viola | SHARK ATTACK</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Alessio Debiasi | Mai una gioia</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Sebastiano Zoller team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2353,6 +2353,38 @@
         </is>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Sebastiano Zoller</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Lorenzo Canali | CGB Gamberoni</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Sebastiano Zoller | CGB Gamberoni</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Andrea  Roveda  | Pinguini Trentini</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Michele Merighi | Clitoriders</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Alessio Debiasi | Mai una gioia</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Gabriele Gottardi team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2385,6 +2385,38 @@
         </is>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Gabriele Gottardi</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Federico Zoller | GREP</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Andrea  Roveda  | Pinguini Trentini</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Luca Perenzoni | CGB Gamberoni</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Michele Merighi | Clitoriders</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Alessio  Giordano  | FC Schalke 104</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Riccardo Barbiero team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2513,6 +2513,38 @@
         </is>
       </c>
     </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Riccardo Barbiero</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Elia Battisti | U.SGUARNA</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Riccardo Barbiero | Rita Levi’s</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Leonardo Viola | SHARK ATTACK</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Marco Sala | IMONTAGNA</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Moris Benedetti | Gli Introvabili</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: fixed player and teams names
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -980,22 +980,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Attila</t>
+          <t>Gennaro Bullo</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Lorenzo Canali | CGB Gamberoni</t>
+          <t>Raffaele Prezzi  | Hellas Lazio</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Nadir  chtioui | Mai una gioia</t>
+          <t>Andrea Conzatti | FC SAVIGNANO</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Andrea Menolli | SdrumALA</t>
+          <t>Alessio Bragagna | SHARK ATTACK</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1005,19 +1005,19 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Alessio Bragagna | SHARK ATTACK</t>
+          <t>Mattia Bertolini | QUEI STRAZI</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Gennaro Bullo</t>
+          <t>Zó</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Raffaele Prezzi  | Hellas Lazio</t>
+          <t>Alberto Cerisara | SHARK ATTACK</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1027,56 +1027,56 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Alessio Bragagna | SHARK ATTACK</t>
+          <t>Federico Nicolodi | U.SGUARNA</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Filippo Benetti | I Magnifici</t>
+          <t>Thomas Perenzoni | CGB Gamberoni</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Mattia Bertolini | QUEI STRAZI</t>
+          <t>Riccardo baldo | wanda tim</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Zó</t>
+          <t>Tommibega</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Alberto Cerisara | SHARK ATTACK</t>
+          <t>Samuele Kettmaier | A.C.DENTI</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Andrea Conzatti | FC SAVIGNANO</t>
+          <t>Andrea Menolli | SdrumALA</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Federico Nicolodi | U.SGUARNA</t>
+          <t>Luca Frasca | Clitoriders</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Thomas Perenzoni | CGB Gamberoni</t>
+          <t>Carlo  Stedile | Mai una gioia</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Riccardo baldo | wanda tim</t>
+          <t>Sayf Brik | A.C.DENTI</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Tommibega</t>
+          <t>APERITIVO AL MOZART</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1086,509 +1086,509 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>Andrea Conzatti | FC SAVIGNANO</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
           <t>Andrea Menolli | SdrumALA</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Luca Frasca | Clitoriders</t>
-        </is>
-      </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Carlo  Stedile | Mai una gioia</t>
+          <t>Giacomo  Gasparini  | Mai una gioia</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Sayf Brik | A.C.DENTI</t>
+          <t>Alessio Zandonai | SBARX</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Tommibega</t>
+          <t>Biker mice</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Samuele Kettmaier | A.C.DENTI</t>
+          <t>Nicolas Giordani  | FC SAVIGNANO</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Andrea Menolli | SdrumALA</t>
+          <t>Federico Fasanelli | SBARX</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Luca Frasca | Clitoriders</t>
+          <t>Matteo Diener | U.SGUARNA</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Carlo  Stedile | Mai una gioia</t>
+          <t>Filippo Benetti | I Magnifici</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Sayf Brik | A.C.DENTI</t>
+          <t>Alessio Debiasi | Mai una gioia</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>APERITIVO AL MOZART</t>
+          <t>Niccoló Orsi</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Samuele Kettmaier | A.C.DENTI</t>
+          <t>Lorenzo Canali | CGB Gamberoni</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Andrea Conzatti | FC SAVIGNANO</t>
+          <t>Alessio Bragagna | SHARK ATTACK</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Andrea Menolli | SdrumALA</t>
+          <t>Nicholas Marzadro | SBARX</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Giacomo  Gasparini  | Mai una gioia</t>
+          <t>Marco Sartorelli | Modium</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Alessio Zandonai | SBARX</t>
+          <t>Mattia Tezzele | U.SGUARNA</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>APERITIVO AL MOZART</t>
+          <t xml:space="preserve">ah ma è ronco </t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Samuele Kettmaier | A.C.DENTI</t>
+          <t>Matteo Zanlucchi | SBARX</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Andrea Conzatti | FC SAVIGNANO</t>
+          <t>Carlo  Stedile | Mai una gioia</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Andrea Menolli | SdrumALA</t>
+          <t>Nicolo  Speziali | FC GORILLAZ</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Giacomo  Gasparini  | Mai una gioia</t>
+          <t>Matteo Simoncelli | IMONTAGNA</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Alessio Zandonai | SBARX</t>
+          <t>Francesco Cristoforetti | Vigili del Fusto</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Biker mice</t>
+          <t>Jacopo Chemini</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Nicolas Giordani  | FC SAVIGNANO</t>
+          <t>Stefano  Tita | Clitoriders</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Federico Fasanelli | SBARX</t>
+          <t>Daniel Pedrotti | IMONTAGNA</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Matteo Diener | U.SGUARNA</t>
+          <t>Michele Merighi | Clitoriders</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Filippo Benetti | I Magnifici</t>
+          <t>maikol  azocar | Mai una gioia</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Alessio Debiasi | Mai una gioia</t>
+          <t>Emanuele Toss | 4SINS</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Niccoló Orsi</t>
+          <t>Senia Lucrezia</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Lorenzo Canali | CGB Gamberoni</t>
+          <t>Elia Battisti | U.SGUARNA</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Alessio Bragagna | SHARK ATTACK</t>
+          <t>Daniel Pedrotti | IMONTAGNA</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Nicholas Marzadro | SBARX</t>
+          <t>Michele Merighi | Clitoriders</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Marco Sartorelli | Modium</t>
+          <t>Gabriele Verona | CGB Gamberoni</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Mattia Tezzele | U.SGUARNA</t>
+          <t>Gianni Sala | FC SALAGIARDINI</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t xml:space="preserve">ah ma è ronco </t>
+          <t>Davide Rosà</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Matteo Zanlucchi | SBARX</t>
+          <t>Elia Barozzi | I Magnifici</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Carlo  Stedile | Mai una gioia</t>
+          <t>Alessio Bragagna | SHARK ATTACK</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Nicolo  Speziali | FC GORILLAZ</t>
+          <t>Sebastiano Zoller | CGB Gamberoni</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Matteo Simoncelli | IMONTAGNA</t>
+          <t>Filippo Benetti | I Magnifici</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Francesco Cristoforetti | Vigili del Fusto</t>
+          <t>Mattia Tezzele | U.SGUARNA</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Jacopo Chemini</t>
+          <t>Nazarena Raos</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Stefano  Tita | Clitoriders</t>
+          <t>Alberto Cerisara | SHARK ATTACK</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Daniel Pedrotti | IMONTAGNA</t>
+          <t>Andrea Gober | U.SGUARNA</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Michele Merighi | Clitoriders</t>
+          <t>Roberto Barozzi | demobusters</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>maikol  azocar | Mai una gioia</t>
+          <t>Andrea Conzatti | FC SAVIGNANO</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Emanuele Toss | 4SINS</t>
+          <t>Gabriele Lasta | RSA United</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Senia Lucrezia</t>
+          <t>LORENZA SIMONCELLI</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Elia Battisti | U.SGUARNA</t>
+          <t>Riccardo Versini | Modium</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Daniel Pedrotti | IMONTAGNA</t>
+          <t>Davide Simoncelli | Avanzi</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Michele Merighi | Clitoriders</t>
+          <t>Carlo  Stedile | Mai una gioia</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Gabriele Verona | CGB Gamberoni</t>
+          <t>Federico Fasanelli | SBARX</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Gianni Sala | FC SALAGIARDINI</t>
+          <t>Emanuele Miorandi | Rita Levi’s</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Davide Rosà</t>
+          <t>Thomas Cavagna</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Elia Barozzi | I Magnifici</t>
+          <t>Thomas Debiasi | Mai una gioia</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Alessio Bragagna | SHARK ATTACK</t>
+          <t>Thomas Cavagna | Mai una gioia</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Sebastiano Zoller | CGB Gamberoni</t>
+          <t>Luca Frasca | Clitoriders</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Filippo Benetti | I Magnifici</t>
+          <t>Federico Nicolodi | U.SGUARNA</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Mattia Tezzele | U.SGUARNA</t>
+          <t>Davide  Bazzano | IMONTAGNA</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Nazarena Raos</t>
+          <t>Nicholas Marzadro</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Alberto Cerisara | SHARK ATTACK</t>
+          <t>Matteo Zanlucchi | SBARX</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Andrea Gober | U.SGUARNA</t>
+          <t>Matteo Diener | U.SGUARNA</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Roberto Barozzi | demobusters</t>
+          <t>Federico Manica | IMONTAGNA</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Andrea Conzatti | FC SAVIGNANO</t>
+          <t>Filippo Benetti | I Magnifici</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Gabriele Lasta | RSA United</t>
+          <t>Alessandro Fanti | FC SALAGIARDINI</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>LORENZA SIMONCELLI</t>
+          <t xml:space="preserve">Valentina Perghem </t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Riccardo Versini | Modium</t>
+          <t>Matteo Zanlucchi | SBARX</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Davide Simoncelli | Avanzi</t>
+          <t>Luca Frasca | Clitoriders</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Carlo  Stedile | Mai una gioia</t>
+          <t>Alessio Bragagna | SHARK ATTACK</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Federico Fasanelli | SBARX</t>
+          <t>Michele Leonardi | Rita Levi’s</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Emanuele Miorandi | Rita Levi’s</t>
+          <t>Matteo Giovannella | Bevem4tut</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Thomas Cavagna</t>
+          <t>Emanuele Miorandi</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Thomas Debiasi | Mai una gioia</t>
+          <t>Alberto Cerisara | SHARK ATTACK</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Thomas Cavagna | Mai una gioia</t>
+          <t>Alessio Bragagna | SHARK ATTACK</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Luca Frasca | Clitoriders</t>
+          <t>Filippo Benetti | I Magnifici</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Federico Nicolodi | U.SGUARNA</t>
+          <t>Alessandro Maffei | FC SAVIGNANO</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Davide  Bazzano | IMONTAGNA</t>
+          <t>Moris Benedetti | Gli Introvabili</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Nicholas Marzadro</t>
+          <t>Jasmine Scottini</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Matteo Zanlucchi | SBARX</t>
+          <t>Elia Battisti | U.SGUARNA</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Matteo Diener | U.SGUARNA</t>
+          <t>Federico Fasanelli | SBARX</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Federico Manica | IMONTAGNA</t>
+          <t>Filippo Benetti | I Magnifici</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Filippo Benetti | I Magnifici</t>
+          <t>Luca Frasca | Clitoriders</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Alessandro Fanti | FC SALAGIARDINI</t>
+          <t>Francesco Cristoforetti | Vigili del Fusto</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Valentina Perghem </t>
+          <t xml:space="preserve">Michele Leonardi </t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Matteo Zanlucchi | SBARX</t>
+          <t>Elia Battisti | U.SGUARNA</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Luca Frasca | Clitoriders</t>
+          <t>Filippo Benetti | I Magnifici</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Alessio Bragagna | SHARK ATTACK</t>
+          <t>Matteo Diener | U.SGUARNA</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Michele Leonardi | Rita Levi’s</t>
+          <t>Luca Tonolli | Rita Levi’s</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Matteo Giovannella | Bevem4tut</t>
+          <t>Sayf Brik | A.C.DENTI</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Emanuele Miorandi</t>
+          <t xml:space="preserve">Mattia Spagnolli </t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Alberto Cerisara | SHARK ATTACK</t>
+          <t>Lorenzo Canali | CGB Gamberoni</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Alessio Bragagna | SHARK ATTACK</t>
+          <t>Filippo Benetti | I Magnifici</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Filippo Benetti | I Magnifici</t>
+          <t>Riccardo Zaffoni | U.SGUARNA</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Alessandro Maffei | FC SAVIGNANO</t>
+          <t>Sebastiano Zoller | CGB Gamberoni</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Moris Benedetti | Gli Introvabili</t>
+          <t>Andrea Giordani | Clitoriders</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Jasmine Scottini</t>
+          <t>Nicolas Giordani</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1598,98 +1598,98 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Federico Fasanelli | SBARX</t>
+          <t>Filippo Benetti | I Magnifici</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Filippo Benetti | I Magnifici</t>
+          <t>Federico Mortillaro | Clitoriders</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Luca Frasca | Clitoriders</t>
+          <t>Federico  Zanini | A.C.DENTI</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Francesco Cristoforetti | Vigili del Fusto</t>
+          <t>Geremia  Carollo | FC SAVIGNANO</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Michele Leonardi </t>
+          <t>Michela Menghini</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Elia Battisti | U.SGUARNA</t>
+          <t>Nicolas Giordani  | FC SAVIGNANO</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Filippo Benetti | I Magnifici</t>
+          <t>Andrea Conzatti | FC SAVIGNANO</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Matteo Diener | U.SGUARNA</t>
+          <t>Matteo Mazzola | GREP</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Luca Tonolli | Rita Levi’s</t>
+          <t>Alessio Farinati | Pinguini Trentini</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Sayf Brik | A.C.DENTI</t>
+          <t>Emanuele  valduga | wanda tim</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mattia Spagnolli </t>
+          <t>JR</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Lorenzo Canali | CGB Gamberoni</t>
+          <t>Elia Battisti | U.SGUARNA</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Filippo Benetti | I Magnifici</t>
+          <t>Luca Tonolli | Rita Levi’s</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Riccardo Zaffoni | U.SGUARNA</t>
+          <t>Alessio Bragagna | SHARK ATTACK</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Sebastiano Zoller | CGB Gamberoni</t>
+          <t>Federico Nicolodi | U.SGUARNA</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Andrea Giordani | Clitoriders</t>
+          <t>Lorenzo Mori` | Hellas Lazio</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Nicolas Giordani</t>
+          <t>Anna Zandonati</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Elia Battisti | U.SGUARNA</t>
+          <t>Nicolas Giordani  | FC SAVIGNANO</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1699,248 +1699,248 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Federico Mortillaro | Clitoriders</t>
+          <t>Federico Fasanelli | SBARX</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Federico  Zanini | A.C.DENTI</t>
+          <t>Luca Frasca | Clitoriders</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Geremia  Carollo | FC SAVIGNANO</t>
+          <t>Alessio Debiasi | Mai una gioia</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Michela Menghini</t>
+          <t>Matteo Alberti</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Nicolas Giordani  | FC SAVIGNANO</t>
+          <t>Thomas Debiasi | Mai una gioia</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Andrea Conzatti | FC SAVIGNANO</t>
+          <t>Nadir  chtioui | Mai una gioia</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Matteo Mazzola | GREP</t>
+          <t>Michael Bertè  | A.C.DENTI</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Alessio Farinati | Pinguini Trentini</t>
+          <t>Andreas Galli | SdrumALA</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Emanuele  valduga | wanda tim</t>
+          <t>Lorenzo Zuani | I Magnifici</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>JR</t>
+          <t xml:space="preserve">Leo Parisi </t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Elia Battisti | U.SGUARNA</t>
+          <t>Daniele Dalbosco | IMONTAGNA</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Luca Tonolli | Rita Levi’s</t>
+          <t>Leonardo Viola | SHARK ATTACK</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Alessio Bragagna | SHARK ATTACK</t>
+          <t>Geremia  Carollo | FC SAVIGNANO</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Federico Nicolodi | U.SGUARNA</t>
+          <t>Luca Frasca | Clitoriders</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Lorenzo Mori` | Hellas Lazio</t>
+          <t>Moris Benedetti | Gli Introvabili</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Anna Zandonati</t>
+          <t>Giacomo Gasparini</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Nicolas Giordani  | FC SAVIGNANO</t>
+          <t>Mattia Kaiserman | Gli Introvabili</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Filippo Benetti | I Magnifici</t>
+          <t>Federico  Andreis | IMONTAGNA</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Federico Fasanelli | SBARX</t>
+          <t>Michele Merighi | Clitoriders</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Luca Frasca | Clitoriders</t>
+          <t>Geremia  Carollo | FC SAVIGNANO</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Alessio Debiasi | Mai una gioia</t>
+          <t>Alessio Delli Compagni | SdrumALA</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Matteo Alberti</t>
+          <t>I magnifici 2.0</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Thomas Debiasi | Mai una gioia</t>
+          <t>Stefano  Tita | Clitoriders</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Nadir  chtioui | Mai una gioia</t>
+          <t>Alessio Bragagna | SHARK ATTACK</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Michael Bertè  | A.C.DENTI</t>
+          <t>Pietro  Gasparini | Mai una gioia</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Andreas Galli | SdrumALA</t>
+          <t>Geremia  Carollo | FC SAVIGNANO</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Lorenzo Zuani | I Magnifici</t>
+          <t>Mattia Tezzele | U.SGUARNA</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Leo Parisi </t>
+          <t>Raffaele Prezzi</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Daniele Dalbosco | IMONTAGNA</t>
+          <t>Thomas Debiasi | Mai una gioia</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Leonardo Viola | SHARK ATTACK</t>
+          <t>Alessio Bragagna | SHARK ATTACK</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Geremia  Carollo | FC SAVIGNANO</t>
+          <t>Sebastiano Zoller | CGB Gamberoni</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Luca Frasca | Clitoriders</t>
+          <t>Andreas Galli | SdrumALA</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Moris Benedetti | Gli Introvabili</t>
+          <t>Mattia Tezzele | U.SGUARNA</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Leo Parisi </t>
+          <t>Danny Giordani</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Daniele Dalbosco | IMONTAGNA</t>
+          <t>Nicolas Giordani  | FC SAVIGNANO</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Leonardo Viola | SHARK ATTACK</t>
+          <t>Danny Giordani | I Magnifici</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Geremia  Carollo | FC SAVIGNANO</t>
+          <t>Luca Frasca | Clitoriders</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Luca Frasca | Clitoriders</t>
+          <t>Alessandro Maffei | FC SAVIGNANO</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Moris Benedetti | Gli Introvabili</t>
+          <t>Gentian Capa | Power Ginger</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Giacomo Gasparini</t>
+          <t>Daniele Ruzzenenti</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Mattia Kaiserman | Gli Introvabili</t>
+          <t>Elia Battisti | U.SGUARNA</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Federico  Andreis | IMONTAGNA</t>
+          <t>Michele Merighi | Clitoriders</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Michele Merighi | Clitoriders</t>
+          <t>Giacomo  Gasparini  | Mai una gioia</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Geremia  Carollo | FC SAVIGNANO</t>
+          <t>Manuel Emanuelli | SdrumALA</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Alessio Delli Compagni | SdrumALA</t>
+          <t>Moris Benedetti | Gli Introvabili</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>I magnifici 2.0</t>
+          <t>Giovanni Simoncelli</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1950,231 +1950,231 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Alessio Bragagna | SHARK ATTACK</t>
+          <t>Daniele Feltrinelli | Rita Levi’s</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Pietro  Gasparini | Mai una gioia</t>
+          <t>Sebastiano Zoller | CGB Gamberoni</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Geremia  Carollo | FC SAVIGNANO</t>
+          <t>Andrea  Pedrotti | IMONTAGNA</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Mattia Tezzele | U.SGUARNA</t>
+          <t>Alessandro Galvagni | Hellas Lazio</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Raffaele Prezzi</t>
+          <t>Riccardo Briosi</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Thomas Debiasi | Mai una gioia</t>
+          <t>Riccardo Versini | Modium</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Alessio Bragagna | SHARK ATTACK</t>
+          <t>Andrea Conzatti | FC SAVIGNANO</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Sebastiano Zoller | CGB Gamberoni</t>
+          <t>Luca Frasca | Clitoriders</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Andreas Galli | SdrumALA</t>
+          <t>Gianni Sala | FC SALAGIARDINI</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Mattia Tezzele | U.SGUARNA</t>
+          <t>Christian Torboli | 4SINS</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Danny Giordani</t>
+          <t>Francesco Passuello</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Nicolas Giordani  | FC SAVIGNANO</t>
+          <t>Gabriel Melis | demobusters</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Danny Giordani | I Magnifici</t>
+          <t>Mattia Baldessarini | SHARK ATTACK</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Luca Frasca | Clitoriders</t>
+          <t>Federico Mortillaro | Clitoriders</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Alessandro Maffei | FC SAVIGNANO</t>
+          <t>Mattia Tezzele | U.SGUARNA</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Gentian Capa | Power Ginger</t>
+          <t>Thomas Pontillo | Gli Introvabili</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Daniele Ruzzenenti</t>
+          <t>Feltri</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Elia Battisti | U.SGUARNA</t>
+          <t>Alberto Cerisara | SHARK ATTACK</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Michele Merighi | Clitoriders</t>
+          <t>Federico  Zanini | A.C.DENTI</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Giacomo  Gasparini  | Mai una gioia</t>
+          <t>Alessio Bragagna | SHARK ATTACK</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Manuel Emanuelli | SdrumALA</t>
+          <t>Filippo Benetti | I Magnifici</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Moris Benedetti | Gli Introvabili</t>
+          <t>Andrea Giordani | Clitoriders</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Giovanni Simoncelli</t>
+          <t>Benny</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Stefano  Tita | Clitoriders</t>
+          <t>Matteo Pilati | Pinguini Trentini</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Daniele Feltrinelli | Rita Levi’s</t>
+          <t>Matteo Simoncelli | IMONTAGNA</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Sebastiano Zoller | CGB Gamberoni</t>
+          <t>Alessio Bragagna | SHARK ATTACK</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Andrea  Pedrotti | IMONTAGNA</t>
+          <t>Riccardo Barbiero | Rita Levi’s</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Alessandro Galvagni | Hellas Lazio</t>
+          <t>Andrea Giordani | Clitoriders</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Riccardo Briosi</t>
+          <t xml:space="preserve">Carlotta </t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Riccardo Versini | Modium</t>
+          <t>Daniele Dalbosco | IMONTAGNA</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Andrea Conzatti | FC SAVIGNANO</t>
+          <t>Andrea Bellini | Nazzzionale ferrovieri</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Luca Frasca | Clitoriders</t>
+          <t>Luca Giordani | SHARK ATTACK</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Gianni Sala | FC SALAGIARDINI</t>
+          <t>Federico  Andreis | IMONTAGNA</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Christian Torboli | 4SINS</t>
+          <t>Andrea Anzelini | GREP</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Francesco Passuello</t>
+          <t>Bruno 🐻</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Gabriel Melis | demobusters</t>
+          <t>Nicolas Giordani  | FC SAVIGNANO</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Mattia Baldessarini | SHARK ATTACK</t>
+          <t>Marco Sala | IMONTAGNA</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Federico Mortillaro | Clitoriders</t>
+          <t>Danny Giordani | I Magnifici</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Mattia Tezzele | U.SGUARNA</t>
+          <t>Riccardo Zaffoni | U.SGUARNA</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Thomas Pontillo | Gli Introvabili</t>
+          <t>Alessio Debiasi | Mai una gioia</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Feltri</t>
+          <t>Davide Scarperi</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Alberto Cerisara | SHARK ATTACK</t>
+          <t>Alessandro  Ruele  | FC GORILLAZ</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Federico  Zanini | A.C.DENTI</t>
+          <t>Andrea Conzatti | FC SAVIGNANO</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -2184,394 +2184,202 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Filippo Benetti | I Magnifici</t>
+          <t>Daniel Pedrotti | IMONTAGNA</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Andrea Giordani | Clitoriders</t>
+          <t>Emanuele  valduga | wanda tim</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Benny</t>
+          <t xml:space="preserve">Davide Raffaelli </t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Matteo Pilati | Pinguini Trentini</t>
+          <t>Alberto Cerisara | SHARK ATTACK</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
+          <t>Daniele Feller | GREP</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
           <t>Matteo Simoncelli | IMONTAGNA</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>Alessio Bragagna | SHARK ATTACK</t>
-        </is>
-      </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Riccardo Barbiero | Rita Levi’s</t>
+          <t>Leonardo Viola | SHARK ATTACK</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Andrea Giordani | Clitoriders</t>
+          <t>Alessio Debiasi | Mai una gioia</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t xml:space="preserve">Carlotta </t>
+          <t>Sebastiano Zoller</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Daniele Dalbosco | IMONTAGNA</t>
+          <t>Lorenzo Canali | CGB Gamberoni</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Andrea Bellini | Nazzzionale ferrovieri</t>
+          <t>Sebastiano Zoller | CGB Gamberoni</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Luca Giordani | SHARK ATTACK</t>
+          <t>Andrea  Roveda  | Pinguini Trentini</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Federico  Andreis | IMONTAGNA</t>
+          <t>Michele Merighi | Clitoriders</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Andrea Anzelini | GREP</t>
+          <t>Alessio Debiasi | Mai una gioia</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Bruno 🐻</t>
+          <t>Gabriele Gottardi</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Nicolas Giordani  | FC SAVIGNANO</t>
+          <t>Federico Zoller | GREP</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Marco Sala | IMONTAGNA</t>
+          <t>Andrea  Roveda  | Pinguini Trentini</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Danny Giordani | I Magnifici</t>
+          <t>Luca Perenzoni | CGB Gamberoni</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Riccardo Zaffoni | U.SGUARNA</t>
+          <t>Michele Merighi | Clitoriders</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Alessio Debiasi | Mai una gioia</t>
+          <t>Alessio  Giordano  | FC Schalke 104</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Davide Scarperi</t>
+          <t>Riccardo Zeni</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Alessandro  Ruele  | FC GORILLAZ</t>
+          <t>Elia Barozzi | I Magnifici</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Andrea Conzatti | FC SAVIGNANO</t>
+          <t>Sebastiano Zoller | CGB Gamberoni</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Alessio Bragagna | SHARK ATTACK</t>
+          <t>Leonardo Viola | SHARK ATTACK</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Daniel Pedrotti | IMONTAGNA</t>
+          <t>Andrea  Roveda  | Pinguini Trentini</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Emanuele  valduga | wanda tim</t>
+          <t>Davide  Bazzano | IMONTAGNA</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Davide Raffaelli </t>
+          <t>Davide Zeni</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Alberto Cerisara | SHARK ATTACK</t>
+          <t>Lorenzo Canali | CGB Gamberoni</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Daniele Feller | GREP</t>
+          <t>Andrea  Roveda  | Pinguini Trentini</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Matteo Simoncelli | IMONTAGNA</t>
+          <t>Alessio Bragagna | SHARK ATTACK</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Leonardo Viola | SHARK ATTACK</t>
+          <t>Luca Perenzoni | CGB Gamberoni</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Alessio Debiasi | Mai una gioia</t>
+          <t>Jacopo  Chemini | IMONTAGNA</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Sebastiano Zoller</t>
+          <t>Riccardo Barbiero</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Lorenzo Canali | CGB Gamberoni</t>
+          <t>Elia Battisti | U.SGUARNA</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Sebastiano Zoller | CGB Gamberoni</t>
+          <t>Riccardo Barbiero | Rita Levi’s</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Andrea  Roveda  | Pinguini Trentini</t>
+          <t>Leonardo Viola | SHARK ATTACK</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Michele Merighi | Clitoriders</t>
+          <t>Marco Sala | IMONTAGNA</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
-        <is>
-          <t>Alessio Debiasi | Mai una gioia</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>Gabriele Gottardi</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>Federico Zoller | GREP</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>Andrea  Roveda  | Pinguini Trentini</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>Luca Perenzoni | CGB Gamberoni</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>Michele Merighi | Clitoriders</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>Alessio  Giordano  | FC Schalke 104</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>Riccardo Zeni</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>Elia Barozzi | I Magnifici</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>Sebastiano Zoller | CGB Gamberoni</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>Leonardo Viola | SHARK ATTACK</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>Andrea  Roveda  | Pinguini Trentini</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>Davide  Bazzano | IMONTAGNA</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>Riccardo Zeni</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>Elia Barozzi | I Magnifici</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>Sebastiano Zoller | CGB Gamberoni</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>Leonardo Viola | SHARK ATTACK</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>Andrea  Roveda  | Pinguini Trentini</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>Davide  Bazzano | IMONTAGNA</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>Davide Zeni</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>Lorenzo Canali | CGB Gamberoni</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>Andrea  Roveda  | Pinguini Trentini</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>Alessio Bragagna | SHARK ATTACK</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>Luca Perenzoni | CGB Gamberoni</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>Jacopo  Chemini | IMONTAGNA</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>Riccardo Barbiero</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>Elia Battisti | U.SGUARNA</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>Riccardo Barbiero | Rita Levi’s</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>Leonardo Viola | SHARK ATTACK</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>Marco Sala | IMONTAGNA</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>Moris Benedetti | Gli Introvabili</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>Riccardo Barbiero</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>Elia Battisti | U.SGUARNA</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>Riccardo Barbiero | Rita Levi’s</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>Leonardo Viola | SHARK ATTACK</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>Marco Sala | IMONTAGNA</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
         <is>
           <t>Moris Benedetti | Gli Introvabili</t>
         </is>

</xml_diff>

<commit_message>
Added Casa 🌫️ team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2385,6 +2385,38 @@
         </is>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Casa 🌫️</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Christian Martinelli | SdrumALA</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Marco Sala | IMONTAGNA</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Nadir Chtioui | Mai una gioia</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Andrea Roveda | Pinguini Trentini</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Stefano Mattioli | SdrumALA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Aste Andrea  team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2417,6 +2417,38 @@
         </is>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Aste Andrea </t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Matteo Pilati | Pinguini Trentini</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Andrea Roveda | Pinguini Trentini</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Alessio Bragagna | SHARK ATTACK</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Edoardo Pomarolli | Modium</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Matteo Maraner | GREP</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Debiasi Alessio team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2481,6 +2481,38 @@
         </is>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Debiasi Alessio</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Elia Battisti | U.SGUARNA</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Michele Merighi | Clitoriders</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Amedeo Malesardi | FC SAVIGNANO</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Federico Nicolodi | U.SGUARNA</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Alessio Debiasi | Mai una gioia</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Matteo pilati team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2577,6 +2577,38 @@
         </is>
       </c>
     </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Matteo pilati</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Elia Battisti | U.SGUARNA</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Michele Merighi | Clitoriders</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Matteo Diener | U.SGUARNA</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Moris Benedetti | Gli Introvabili</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Emiliano Bici | Power Ginger</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Elia tomasoni  team
</commit_message>
<xml_diff>
--- a/assets/2025/squadre.xlsx
+++ b/assets/2025/squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2609,6 +2609,38 @@
         </is>
       </c>
     </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Elia tomasoni </t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Stefano Tita | Clitoriders</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Luca Frasca | Clitoriders</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Giovanni Giusto | demobusters</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Saverio Santoro | U.SGUARNA</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Moris Benedetti | Gli Introvabili</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>